<commit_message>
Update 1/3/23 Database changes Add RunLog - API and APP
</commit_message>
<xml_diff>
--- a/RavenDB/DataFiles/DistillationTables.xlsx
+++ b/RavenDB/DataFiles/DistillationTables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBeck\WorkDB\RLRMDB\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBeck\Raven\RavenDB\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1623C33-0BBA-4212-8570-3C10ECE1B97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06818B3C-D06F-4F26-84CC-2B586D64E822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3504" yWindow="1284" windowWidth="18900" windowHeight="10248" firstSheet="3" activeTab="5" xr2:uid="{8FD5DCFB-4924-4DCA-A219-158A02B80ACB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="9" xr2:uid="{8FD5DCFB-4924-4DCA-A219-158A02B80ACB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="338">
   <si>
     <t>RUN LOG</t>
   </si>
@@ -2016,10 +2016,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB46B176-E83F-48DE-A71A-A4D66EAEBE3A}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2027,11 +2027,10 @@
     <col min="2" max="2" width="26.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>332</v>
       </c>
@@ -2045,13 +2044,10 @@
         <v>187</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>335</v>
       </c>
@@ -2064,13 +2060,12 @@
       <c r="D2" s="5">
         <v>-190</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5">
+      <c r="E2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>335</v>
       </c>
@@ -2083,13 +2078,12 @@
       <c r="D3" s="5">
         <v>-20</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>335</v>
       </c>
@@ -2102,13 +2096,12 @@
       <c r="D4" s="5">
         <v>0.16</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5">
+      <c r="E4" s="5">
         <v>0.2</v>
       </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>335</v>
       </c>
@@ -2121,13 +2114,12 @@
       <c r="D5" s="5">
         <v>0.25</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5">
+      <c r="E5" s="5">
         <v>0.2</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>335</v>
       </c>
@@ -2140,13 +2132,12 @@
       <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5">
+      <c r="E6" s="5">
         <v>0.5</v>
       </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>335</v>
       </c>
@@ -2159,13 +2150,12 @@
       <c r="D7" s="5">
         <v>15</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5">
+      <c r="E7" s="5">
         <v>4</v>
       </c>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>335</v>
       </c>
@@ -2178,13 +2168,12 @@
       <c r="D8" s="5">
         <v>15</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5">
+      <c r="E8" s="5">
         <v>3</v>
       </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>335</v>
       </c>
@@ -2197,13 +2186,12 @@
       <c r="D9" s="5">
         <v>17</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5">
+      <c r="E9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>335</v>
       </c>
@@ -2216,13 +2204,12 @@
       <c r="D10" s="5">
         <v>20</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5">
+      <c r="E10" s="5">
         <v>3</v>
       </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>335</v>
       </c>
@@ -2235,13 +2222,12 @@
       <c r="D11" s="5">
         <v>27</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5">
+      <c r="E11" s="5">
         <v>20</v>
       </c>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>335</v>
       </c>
@@ -2254,14 +2240,13 @@
       <c r="D12" s="5">
         <v>40</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5">
+      <c r="E12" s="5">
         <v>20</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>335</v>
       </c>
@@ -2274,13 +2259,12 @@
       <c r="D13" s="5">
         <v>43</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5">
+      <c r="E13" s="5">
         <v>20</v>
       </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>335</v>
       </c>
@@ -2293,13 +2277,12 @@
       <c r="D14" s="5">
         <v>125</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5">
+      <c r="E14" s="5">
         <v>2</v>
       </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>335</v>
       </c>
@@ -2312,13 +2295,12 @@
       <c r="D15" s="5">
         <v>125</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5">
+      <c r="E15" s="5">
         <v>5</v>
       </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>335</v>
       </c>
@@ -2331,13 +2313,12 @@
       <c r="D16" s="5">
         <v>160</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5">
+      <c r="E16" s="5">
         <v>3</v>
       </c>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>335</v>
       </c>
@@ -2350,13 +2331,12 @@
       <c r="D17" s="5">
         <v>170</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5">
+      <c r="E17" s="5">
         <v>20</v>
       </c>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>335</v>
       </c>
@@ -2369,13 +2349,12 @@
       <c r="D18" s="5">
         <v>175</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5">
+      <c r="E18" s="5">
         <v>3</v>
       </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>335</v>
       </c>
@@ -2388,13 +2367,12 @@
       <c r="D19" s="5">
         <v>190</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5">
+      <c r="E19" s="5">
         <v>10</v>
       </c>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>335</v>
       </c>
@@ -2407,13 +2385,12 @@
       <c r="D20" s="5">
         <v>210</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5">
+      <c r="E20" s="5">
         <v>20</v>
       </c>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>335</v>
       </c>
@@ -2426,130 +2403,84 @@
       <c r="D21" s="5">
         <v>220</v>
       </c>
-      <c r="F21" s="5">
+      <c r="E21" s="5">
         <v>20</v>
       </c>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>335</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="D22" s="5">
-        <v>232</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="5">
-        <v>10</v>
-      </c>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>335</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D23" s="5">
-        <v>242</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="5">
-        <v>10</v>
-      </c>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>335</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>335</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>105</v>
-      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>335</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>110</v>
-      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="6"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B28" s="6"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="6"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L31">
-    <sortCondition ref="D2:D31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K29">
+    <sortCondition ref="D2:D29"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4512,8 +4443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B241E7-4B79-4B7D-8314-F249B1FAF596}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6093,7 +6024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3629CE-C6CA-4B57-8AC8-682D6F2362D9}">
   <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A121" workbookViewId="0">
       <selection activeCell="A97" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -8522,16 +8453,16 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:F26"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>